<commit_message>
Correct 10% to 50% in feedback texts. Update to metadata.
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD36B4F-749E-4E1F-9FF3-668C2DAA8B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17645F03-1C59-4A47-8B96-1D371CCBFAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15225" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="231">
   <si>
     <t>tab_name</t>
   </si>
@@ -721,6 +721,18 @@
   </si>
   <si>
     <t>Rate of Going missing, per 10,000 children</t>
+  </si>
+  <si>
+    <t>Severe absentees for CLA 12 months at 31 March (overall absence 50% or more)</t>
+  </si>
+  <si>
+    <t>Severe absentees for CINO at 31 March (overall absence 50% or more)</t>
+  </si>
+  <si>
+    <t>Severe absentees for CPPO at 31 March (overall absence 50% or more)</t>
+  </si>
+  <si>
+    <t>pt_pupils_pa_50_exact</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J64"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,22 +1549,22 @@
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1567,22 +1579,22 @@
         <v>9</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
+        <v>229</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1597,22 +1609,22 @@
         <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>38</v>
+        <v>227</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>44</v>
+        <v>230</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1630,15 +1642,17 @@
         <v>36</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I17" s="5" t="s">
         <v>136</v>
       </c>
@@ -1658,15 +1672,17 @@
         <v>36</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I18" s="5" t="s">
         <v>137</v>
       </c>
@@ -1686,15 +1702,17 @@
         <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I19" s="5" t="s">
         <v>138</v>
       </c>
@@ -1708,25 +1726,23 @@
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1738,25 +1754,23 @@
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1768,25 +1782,23 @@
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>212</v>
+        <v>36</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1798,25 +1810,25 @@
         <v>6</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>212</v>
+        <v>46</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>13</v>
+        <v>139</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1828,23 +1840,25 @@
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>212</v>
+        <v>46</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>208</v>
+        <v>48</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I24" s="5" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1859,24 +1873,24 @@
         <v>51</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>213</v>
+        <v>52</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="H25" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I25" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>173</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1889,24 +1903,24 @@
         <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>214</v>
+        <v>53</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="H26" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I26" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>176</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -1919,24 +1933,22 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>201</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>177</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1952,7 +1964,7 @@
         <v>114</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>127</v>
@@ -1962,10 +1974,10 @@
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1982,7 +1994,7 @@
         <v>114</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>127</v>
@@ -1992,10 +2004,10 @@
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2012,7 +2024,7 @@
         <v>114</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>127</v>
@@ -2022,10 +2034,10 @@
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>120</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2042,7 +2054,7 @@
         <v>114</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>127</v>
@@ -2052,10 +2064,10 @@
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2072,7 +2084,7 @@
         <v>114</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>127</v>
@@ -2082,10 +2094,10 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2102,7 +2114,7 @@
         <v>114</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>127</v>
@@ -2112,10 +2124,10 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>186</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2132,7 +2144,7 @@
         <v>114</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>127</v>
@@ -2142,10 +2154,10 @@
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2162,7 +2174,7 @@
         <v>114</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>127</v>
@@ -2172,10 +2184,10 @@
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2192,7 +2204,7 @@
         <v>114</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>127</v>
@@ -2202,10 +2214,10 @@
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2219,10 +2231,10 @@
         <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>127</v>
@@ -2232,10 +2244,10 @@
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2249,10 +2261,10 @@
         <v>51</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>127</v>
@@ -2262,10 +2274,10 @@
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2279,10 +2291,10 @@
         <v>51</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>127</v>
@@ -2292,10 +2304,10 @@
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>112</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2312,7 +2324,7 @@
         <v>128</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>127</v>
@@ -2322,10 +2334,10 @@
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2342,7 +2354,7 @@
         <v>128</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>127</v>
@@ -2352,10 +2364,10 @@
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2366,27 +2378,27 @@
         <v>6</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>59</v>
+        <v>206</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J42" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -2396,27 +2408,27 @@
         <v>6</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J43" s="5"/>
+        <v>195</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -2426,25 +2438,27 @@
         <v>6</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>63</v>
+        <v>207</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J44" s="5"/>
+        <v>172</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -2460,19 +2474,19 @@
         <v>61</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J45" s="5"/>
     </row>
@@ -2490,7 +2504,7 @@
         <v>61</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>69</v>
@@ -2502,7 +2516,7 @@
         <v>154</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="J46" s="5"/>
     </row>
@@ -2520,19 +2534,17 @@
         <v>61</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J47" s="5"/>
     </row>
@@ -2547,20 +2559,22 @@
         <v>60</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>162</v>
+        <v>64</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>165</v>
+        <v>69</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="H48" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I48" s="5" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="J48" s="5"/>
     </row>
@@ -2575,13 +2589,13 @@
         <v>60</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>50</v>
@@ -2590,7 +2604,7 @@
         <v>154</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="J49" s="5"/>
     </row>
@@ -2605,13 +2619,13 @@
         <v>60</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>50</v>
@@ -2620,7 +2634,7 @@
         <v>154</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2635,22 +2649,20 @@
         <v>60</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="J51" s="5"/>
     </row>
@@ -2668,10 +2680,10 @@
         <v>70</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>50</v>
@@ -2680,7 +2692,7 @@
         <v>154</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J52" s="5"/>
     </row>
@@ -2689,96 +2701,90 @@
         <v>52</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>202</v>
+        <v>50</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -2791,18 +2797,20 @@
         <v>80</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H56" s="5"/>
+        <v>169</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I56" s="5" t="s">
         <v>13</v>
       </c>
@@ -2821,18 +2829,20 @@
         <v>80</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H57" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="I57" s="5" t="s">
         <v>13</v>
       </c>
@@ -2851,18 +2861,20 @@
         <v>80</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>156</v>
+        <v>88</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H58" s="5"/>
+        <v>202</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I58" s="5" t="s">
         <v>13</v>
       </c>
@@ -2884,13 +2896,13 @@
         <v>90</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>156</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
@@ -2908,23 +2920,21 @@
         <v>79</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>211</v>
+        <v>80</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
         <v>13</v>
       </c>
@@ -2940,23 +2950,21 @@
         <v>79</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>211</v>
+        <v>80</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
         <v>13</v>
       </c>
@@ -2972,23 +2980,21 @@
         <v>79</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>211</v>
+        <v>80</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>154</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
         <v>13</v>
       </c>
@@ -3007,18 +3013,20 @@
         <v>211</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>99</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H63" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="I63" s="5" t="s">
         <v>13</v>
       </c>
@@ -3037,24 +3045,118 @@
         <v>211</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>154</v>
       </c>
       <c r="I64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I67" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J67" s="5" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Raw Data-related changes prior to running pipeline
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17645F03-1C59-4A47-8B96-1D371CCBFAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814AE112-3DF2-401A-A5FC-6FB2E4308CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15225" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -459,9 +459,6 @@
     <t>list('social_care_group' = 'CLA 12 months at 31 March')</t>
   </si>
   <si>
-    <t>list('characteristic' = 'Special guardianship orders')</t>
-  </si>
-  <si>
     <t>list('characteristic' = 'Residence order or child arrangement order granted')</t>
   </si>
   <si>
@@ -733,6 +730,9 @@
   </si>
   <si>
     <t>pt_pupils_pa_50_exact</t>
+  </si>
+  <si>
+    <t>list('characteristic' = 'Special guardianship order')</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1179,13 +1179,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -1239,7 +1239,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>13</v>
@@ -1260,7 +1260,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>19</v>
@@ -1288,7 +1288,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>19</v>
@@ -1316,7 +1316,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -1347,7 +1347,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>23</v>
@@ -1381,7 +1381,7 @@
         <v>32</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>133</v>
@@ -1411,7 +1411,7 @@
         <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>134</v>
@@ -1441,7 +1441,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>135</v>
@@ -1471,7 +1471,7 @@
         <v>33</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>133</v>
@@ -1501,7 +1501,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>134</v>
@@ -1531,7 +1531,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>135</v>
@@ -1552,16 +1552,16 @@
         <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>133</v>
@@ -1582,16 +1582,16 @@
         <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>134</v>
@@ -1612,16 +1612,16 @@
         <v>30</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>135</v>
@@ -1651,7 +1651,7 @@
         <v>44</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>136</v>
@@ -1681,7 +1681,7 @@
         <v>44</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>137</v>
@@ -1711,7 +1711,7 @@
         <v>44</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>138</v>
@@ -1825,10 +1825,10 @@
         <v>50</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>139</v>
+        <v>230</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1855,10 +1855,10 @@
         <v>50</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1873,7 +1873,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>52</v>
@@ -1885,7 +1885,7 @@
         <v>54</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>13</v>
@@ -1903,7 +1903,7 @@
         <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>53</v>
@@ -1915,7 +1915,7 @@
         <v>57</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>13</v>
@@ -1933,10 +1933,10 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>58</v>
@@ -1964,20 +1964,20 @@
         <v>114</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1994,20 +1994,20 @@
         <v>114</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2024,20 +2024,20 @@
         <v>114</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2054,20 +2054,20 @@
         <v>114</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2084,20 +2084,20 @@
         <v>114</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2114,17 +2114,17 @@
         <v>114</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>120</v>
@@ -2144,20 +2144,20 @@
         <v>114</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="J34" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2174,20 +2174,20 @@
         <v>114</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2204,20 +2204,20 @@
         <v>114</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2234,20 +2234,20 @@
         <v>114</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2264,20 +2264,20 @@
         <v>114</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J38" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2294,20 +2294,20 @@
         <v>114</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J39" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2324,20 +2324,20 @@
         <v>128</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2354,20 +2354,20 @@
         <v>128</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2384,17 +2384,17 @@
         <v>128</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>112</v>
@@ -2414,20 +2414,20 @@
         <v>128</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2444,17 +2444,17 @@
         <v>128</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>111</v>
@@ -2483,10 +2483,10 @@
         <v>68</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J45" s="5"/>
     </row>
@@ -2513,10 +2513,10 @@
         <v>50</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J46" s="5"/>
     </row>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J47" s="5"/>
     </row>
@@ -2571,10 +2571,10 @@
         <v>50</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J48" s="5"/>
     </row>
@@ -2601,10 +2601,10 @@
         <v>50</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J49" s="5"/>
     </row>
@@ -2631,10 +2631,10 @@
         <v>50</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2649,20 +2649,20 @@
         <v>60</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="F51" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J51" s="5"/>
     </row>
@@ -2689,10 +2689,10 @@
         <v>50</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J52" s="5"/>
     </row>
@@ -2719,10 +2719,10 @@
         <v>50</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J53" s="5"/>
     </row>
@@ -2749,10 +2749,10 @@
         <v>50</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J54" s="5"/>
     </row>
@@ -2779,10 +2779,10 @@
         <v>50</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J55" s="5"/>
     </row>
@@ -2806,10 +2806,10 @@
         <v>85</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>13</v>
@@ -2841,7 +2841,7 @@
         <v>87</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>13</v>
@@ -2870,10 +2870,10 @@
         <v>88</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>13</v>
@@ -2899,10 +2899,10 @@
         <v>89</v>
       </c>
       <c r="F59" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
@@ -2929,10 +2929,10 @@
         <v>91</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
@@ -2959,10 +2959,10 @@
         <v>92</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
@@ -2989,10 +2989,10 @@
         <v>93</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
@@ -3010,7 +3010,7 @@
         <v>79</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>94</v>
@@ -3025,7 +3025,7 @@
         <v>98</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>13</v>
@@ -3042,7 +3042,7 @@
         <v>79</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>94</v>
@@ -3057,7 +3057,7 @@
         <v>100</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>13</v>
@@ -3074,7 +3074,7 @@
         <v>79</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>94</v>
@@ -3089,7 +3089,7 @@
         <v>101</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>13</v>
@@ -3106,7 +3106,7 @@
         <v>79</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>102</v>
@@ -3136,7 +3136,7 @@
         <v>79</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>105</v>
@@ -3151,13 +3151,13 @@
         <v>108</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I67" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J67" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3187,7 +3187,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -3204,7 +3204,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3221,7 +3221,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -3241,7 +3241,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw data for "Children Looked after at/on 31 March - switched on/at in the input file so we react accordingly in dimensional filters
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814AE112-3DF2-401A-A5FC-6FB2E4308CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BD3518-7836-497A-A70D-3CEB52FF3760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="233">
   <si>
     <t>tab_name</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>list('characteristic' = 'Special guardianship order')</t>
+  </si>
+  <si>
+    <t>list('population_count' = 'Children looked after on 31 March each year')</t>
+  </si>
+  <si>
+    <t>list('population_count' = 'Children looked after on 31 March each year', 'characteristic' = 'UASC')</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1304,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>131</v>
+        <v>231</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -1354,7 +1360,7 @@
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="J7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Metadata update, tidied up indicator text in a couple of places
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BD3518-7836-497A-A70D-3CEB52FF3760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91238871-EA82-4973-B2B7-9D0831C78C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -237,12 +237,6 @@
     <t>% CLA on 31 March living in foster care</t>
   </si>
   <si>
-    <t>% living in secure homes and children's homes</t>
-  </si>
-  <si>
-    <t>% living in independent and semi-independent living arrangements/supported accommodation</t>
-  </si>
-  <si>
     <t>placement_changes_data</t>
   </si>
   <si>
@@ -739,6 +733,12 @@
   </si>
   <si>
     <t>list('population_count' = 'Children looked after on 31 March each year', 'characteristic' = 'UASC')</t>
+  </si>
+  <si>
+    <t>% CLA on 31 March living in secure homes and children's homes</t>
+  </si>
+  <si>
+    <t>% CLA on 31 March living in independent and semi-independent living arrangements/supported accommodation</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1170,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1185,13 +1185,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1208,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -1245,7 +1245,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>13</v>
@@ -1266,7 +1266,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>19</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -1294,7 +1294,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>19</v>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -1322,7 +1322,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -1353,14 +1353,14 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1387,10 +1387,10 @@
         <v>32</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -1417,10 +1417,10 @@
         <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -1447,10 +1447,10 @@
         <v>32</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1477,10 +1477,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -1507,10 +1507,10 @@
         <v>33</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -1537,10 +1537,10 @@
         <v>33</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1558,19 +1558,19 @@
         <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1588,19 +1588,19 @@
         <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1618,19 +1618,19 @@
         <v>30</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1657,10 +1657,10 @@
         <v>44</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J17" s="5"/>
     </row>
@@ -1687,10 +1687,10 @@
         <v>44</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1717,10 +1717,10 @@
         <v>44</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1831,10 +1831,10 @@
         <v>50</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1861,10 +1861,10 @@
         <v>50</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1879,7 +1879,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>52</v>
@@ -1891,7 +1891,7 @@
         <v>54</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>13</v>
@@ -1909,7 +1909,7 @@
         <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>53</v>
@@ -1921,7 +1921,7 @@
         <v>57</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>13</v>
@@ -1939,10 +1939,10 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>58</v>
@@ -1967,23 +1967,23 @@
         <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1997,23 +1997,23 @@
         <v>51</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2027,23 +2027,23 @@
         <v>51</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2057,23 +2057,23 @@
         <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2087,23 +2087,23 @@
         <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2117,23 +2117,23 @@
         <v>51</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2147,23 +2147,23 @@
         <v>51</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2177,23 +2177,23 @@
         <v>51</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2207,23 +2207,23 @@
         <v>51</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2237,23 +2237,23 @@
         <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2267,23 +2267,23 @@
         <v>51</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2297,23 +2297,23 @@
         <v>51</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2327,23 +2327,23 @@
         <v>51</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2357,23 +2357,23 @@
         <v>51</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2387,23 +2387,23 @@
         <v>51</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2417,23 +2417,23 @@
         <v>51</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2447,23 +2447,23 @@
         <v>51</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2483,16 +2483,16 @@
         <v>59</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J45" s="5"/>
     </row>
@@ -2513,16 +2513,16 @@
         <v>62</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J46" s="5"/>
     </row>
@@ -2543,14 +2543,14 @@
         <v>63</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J47" s="5"/>
     </row>
@@ -2571,16 +2571,16 @@
         <v>64</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J48" s="5"/>
     </row>
@@ -2598,19 +2598,19 @@
         <v>61</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J49" s="5"/>
     </row>
@@ -2628,19 +2628,19 @@
         <v>61</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2655,20 +2655,20 @@
         <v>60</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J51" s="5"/>
     </row>
@@ -2683,22 +2683,22 @@
         <v>60</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J52" s="5"/>
     </row>
@@ -2713,22 +2713,22 @@
         <v>60</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="F53" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J53" s="5"/>
     </row>
@@ -2743,22 +2743,22 @@
         <v>60</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J54" s="5"/>
     </row>
@@ -2773,22 +2773,22 @@
         <v>60</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J55" s="5"/>
     </row>
@@ -2797,25 +2797,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="F56" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>13</v>
@@ -2829,25 +2829,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F57" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>13</v>
@@ -2861,25 +2861,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>13</v>
@@ -2893,22 +2893,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
@@ -2923,22 +2923,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F60" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
@@ -2953,22 +2953,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="F61" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
@@ -2983,22 +2983,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
@@ -3013,25 +3013,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>13</v>
@@ -3045,25 +3045,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F64" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>13</v>
@@ -3077,25 +3077,25 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E65" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G65" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="H65" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>13</v>
@@ -3109,22 +3109,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5" t="s">
@@ -3139,31 +3139,31 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="G67" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F67" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="H67" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3193,7 +3193,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -3202,7 +3202,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3210,7 +3210,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3219,7 +3219,7 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3227,7 +3227,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -3236,7 +3236,7 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3247,18 +3247,18 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3381,62 +3381,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3456,27 +3456,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement module for the LA chart and Stats neighbours chart
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BD3518-7836-497A-A70D-3CEB52FF3760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A406B221-903F-4665-848C-08C566C96D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="237">
   <si>
     <t>tab_name</t>
   </si>
@@ -739,6 +739,18 @@
   </si>
   <si>
     <t>list('population_count' = 'Children looked after on 31 March each year', 'characteristic' = 'UASC')</t>
+  </si>
+  <si>
+    <t>Social worker stability</t>
+  </si>
+  <si>
+    <t>sw_stability</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>list('cla_group'='CLA on 31 March','sw_stability'='3 or more social workers during the year')</t>
   </si>
 </sst>
 </file>
@@ -1143,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3145,24 +3157,56 @@
         <v>210</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F68" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G68" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H68" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J67" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SW stability summary page updated and the minor cglitches sorted in outputs
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A406B221-903F-4665-848C-08C566C96D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E210A6-A546-4B49-89B2-87E4965548BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="540" yWindow="315" windowWidth="21105" windowHeight="20520" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="236">
   <si>
     <t>tab_name</t>
   </si>
@@ -741,16 +741,13 @@
     <t>list('population_count' = 'Children looked after on 31 March each year', 'characteristic' = 'UASC')</t>
   </si>
   <si>
-    <t>Social worker stability</t>
-  </si>
-  <si>
-    <t>sw_stability</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>list('cla_group'='CLA on 31 March','sw_stability'='3 or more social workers during the year')</t>
+    <t>list('cla_group' = 'CLA on 31 March', 'sw_stability' = '3 or more social workers during the year')</t>
+  </si>
+  <si>
+    <t>sw_stability_data</t>
+  </si>
+  <si>
+    <t>Percentage of children with 3 or more social workers in past 12 months</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,19 +3157,19 @@
         <v>102</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>234</v>
       </c>
       <c r="G67" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H67" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H67" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="I67" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Update text for sw_stability and get metadata in line with Nat's branch
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E210A6-A546-4B49-89B2-87E4965548BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8977C7EF-FDAE-4A3B-8E35-755033FA237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="315" windowWidth="21105" windowHeight="20520" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -237,12 +237,6 @@
     <t>% CLA on 31 March living in foster care</t>
   </si>
   <si>
-    <t>% living in secure homes and children's homes</t>
-  </si>
-  <si>
-    <t>% living in independent and semi-independent living arrangements/supported accommodation</t>
-  </si>
-  <si>
     <t>placement_changes_data</t>
   </si>
   <si>
@@ -748,6 +742,12 @@
   </si>
   <si>
     <t>Percentage of children with 3 or more social workers in past 12 months</t>
+  </si>
+  <si>
+    <t>% CLA on 31 March living in secure homes and children's homes</t>
+  </si>
+  <si>
+    <t>% CLA on 31 March living in independent and semi-independent living arrangements/supported accommodation</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1194,13 +1194,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -1254,7 +1254,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>13</v>
@@ -1275,7 +1275,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>19</v>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J4" s="5"/>
     </row>
@@ -1303,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>19</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J5" s="5"/>
     </row>
@@ -1331,7 +1331,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -1362,14 +1362,14 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1396,10 +1396,10 @@
         <v>32</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -1426,10 +1426,10 @@
         <v>32</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J9" s="5"/>
     </row>
@@ -1456,10 +1456,10 @@
         <v>32</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J10" s="5"/>
     </row>
@@ -1486,10 +1486,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -1516,10 +1516,10 @@
         <v>33</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -1546,10 +1546,10 @@
         <v>33</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J13" s="5"/>
     </row>
@@ -1567,19 +1567,19 @@
         <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J14" s="5"/>
     </row>
@@ -1597,19 +1597,19 @@
         <v>30</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J15" s="5"/>
     </row>
@@ -1627,19 +1627,19 @@
         <v>30</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J16" s="5"/>
     </row>
@@ -1666,10 +1666,10 @@
         <v>44</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J17" s="5"/>
     </row>
@@ -1696,10 +1696,10 @@
         <v>44</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -1726,10 +1726,10 @@
         <v>44</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J19" s="5"/>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J20" s="5"/>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J21" s="5"/>
     </row>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J22" s="5"/>
     </row>
@@ -1840,10 +1840,10 @@
         <v>50</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J23" s="5"/>
     </row>
@@ -1870,10 +1870,10 @@
         <v>50</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J24" s="5"/>
     </row>
@@ -1888,7 +1888,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>52</v>
@@ -1900,7 +1900,7 @@
         <v>54</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>13</v>
@@ -1918,7 +1918,7 @@
         <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>53</v>
@@ -1930,7 +1930,7 @@
         <v>57</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>13</v>
@@ -1948,10 +1948,10 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>58</v>
@@ -1976,23 +1976,23 @@
         <v>51</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2006,23 +2006,23 @@
         <v>51</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2036,23 +2036,23 @@
         <v>51</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2066,23 +2066,23 @@
         <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2096,23 +2096,23 @@
         <v>51</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2126,23 +2126,23 @@
         <v>51</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2156,23 +2156,23 @@
         <v>51</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2186,23 +2186,23 @@
         <v>51</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2216,23 +2216,23 @@
         <v>51</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2246,23 +2246,23 @@
         <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2276,23 +2276,23 @@
         <v>51</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,23 +2306,23 @@
         <v>51</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2336,23 +2336,23 @@
         <v>51</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2366,23 +2366,23 @@
         <v>51</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2396,23 +2396,23 @@
         <v>51</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2426,23 +2426,23 @@
         <v>51</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2456,23 +2456,23 @@
         <v>51</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2492,16 +2492,16 @@
         <v>59</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J45" s="5"/>
     </row>
@@ -2522,16 +2522,16 @@
         <v>62</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J46" s="5"/>
     </row>
@@ -2552,14 +2552,14 @@
         <v>63</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J47" s="5"/>
     </row>
@@ -2580,16 +2580,16 @@
         <v>64</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J48" s="5"/>
     </row>
@@ -2606,20 +2606,20 @@
       <c r="D49" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>65</v>
+      <c r="E49" t="s">
+        <v>234</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J49" s="5"/>
     </row>
@@ -2636,20 +2636,20 @@
       <c r="D50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>66</v>
+      <c r="E50" t="s">
+        <v>235</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2664,20 +2664,20 @@
         <v>60</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E51" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J51" s="5"/>
     </row>
@@ -2692,22 +2692,22 @@
         <v>60</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J52" s="5"/>
     </row>
@@ -2722,22 +2722,22 @@
         <v>60</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="F53" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J53" s="5"/>
     </row>
@@ -2752,22 +2752,22 @@
         <v>60</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J54" s="5"/>
     </row>
@@ -2782,22 +2782,22 @@
         <v>60</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J55" s="5"/>
     </row>
@@ -2806,25 +2806,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="F56" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>13</v>
@@ -2838,25 +2838,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F57" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>13</v>
@@ -2870,25 +2870,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>13</v>
@@ -2902,22 +2902,22 @@
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5" t="s">
@@ -2932,22 +2932,22 @@
         <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F60" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
@@ -2962,22 +2962,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="F61" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5" t="s">
@@ -2992,22 +2992,22 @@
         <v>61</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5" t="s">
@@ -3022,25 +3022,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>13</v>
@@ -3054,25 +3054,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F64" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>13</v>
@@ -3086,25 +3086,25 @@
         <v>64</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E65" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G65" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="H65" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>13</v>
@@ -3118,22 +3118,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G66" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5" t="s">
@@ -3148,28 +3148,28 @@
         <v>66</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J67" s="5" t="s">
         <v>13</v>
@@ -3180,31 +3180,31 @@
         <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F68" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="G68" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F68" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="H68" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3234,7 +3234,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -3243,7 +3243,7 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3260,7 +3260,7 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -3277,7 +3277,7 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3288,18 +3288,18 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3422,62 +3422,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3497,27 +3497,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update headline text and Summary Page to mention CLA
</commit_message>
<xml_diff>
--- a/data/summary_page_metadata.xlsx
+++ b/data/summary_page_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweller1\Documents\projects\CSC_outcomes_and_enablers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8977C7EF-FDAE-4A3B-8E35-755033FA237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9A3853-D5D3-45C8-8F8A-BE6363504F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
+    <workbookView xWindow="27480" yWindow="60" windowWidth="22080" windowHeight="20520" xr2:uid="{8BE61BC9-B2AB-47B5-AD20-88FB73760243}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcomes" sheetId="1" r:id="rId1"/>
@@ -741,13 +741,13 @@
     <t>sw_stability_data</t>
   </si>
   <si>
-    <t>Percentage of children with 3 or more social workers in past 12 months</t>
-  </si>
-  <si>
     <t>% CLA on 31 March living in secure homes and children's homes</t>
   </si>
   <si>
     <t>% CLA on 31 March living in independent and semi-independent living arrangements/supported accommodation</t>
+  </si>
+  <si>
+    <t>% CLA with 3 or more social workers in past 12 months</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56502052-C975-45FA-BF34-A15F87F5C15F}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2607,7 @@
         <v>61</v>
       </c>
       <c r="E49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>67</v>
@@ -2637,7 +2637,7 @@
         <v>61</v>
       </c>
       <c r="E50" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>67</v>
@@ -3157,7 +3157,7 @@
         <v>100</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>232</v>

</xml_diff>